<commit_message>
Update Microcontroller Team 1.xlsx
</commit_message>
<xml_diff>
--- a/Microcontroller Team 1.xlsx
+++ b/Microcontroller Team 1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\winter20-21\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\HSHL\SOFTWARE FOR ELE\GitHub\winter20-21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D60058A-6A7E-4115-8730-D3A1635A0FDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7F2B52-74CE-4902-98D6-056E6D553059}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,33 +25,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Microcontroller Team 1</t>
   </si>
   <si>
-    <t xml:space="preserve">Muhammad Amirul Hakimi </t>
-  </si>
-  <si>
-    <t>Bin Zaprunnizam</t>
-  </si>
-  <si>
-    <t>Muhammad Amjad</t>
-  </si>
-  <si>
-    <t>Bin Abdul Malik</t>
-  </si>
-  <si>
-    <t>Muhammad Iqbal</t>
-  </si>
-  <si>
-    <t>Bin Mohd Fauzi</t>
-  </si>
-  <si>
-    <t>Muhammad Farid Izwan</t>
-  </si>
-  <si>
-    <t>Bin Mohamad Shabri</t>
+    <t>Muhammad Amirul Hakimi  Bin Zaprunnizam</t>
+  </si>
+  <si>
+    <t>Muhammad Farid Izwan Bin Mohamad Shabri</t>
+  </si>
+  <si>
+    <t>Muhammad Iqbal Bin Mohd Fauzi</t>
+  </si>
+  <si>
+    <t>Muhammad Amjad Bin Abdul Malik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patrick Stephen </t>
+  </si>
+  <si>
+    <t>week</t>
+  </si>
+  <si>
+    <t>Coding for Arduino Circuit Pedestrian &amp;Car traffic light</t>
   </si>
 </sst>
 </file>
@@ -369,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -381,41 +378,45 @@
     <col min="2" max="2" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>